<commit_message>
inclusão de cores e melhorias
</commit_message>
<xml_diff>
--- a/planilha/planilha_teste.xlsx
+++ b/planilha/planilha_teste.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlos.pepato\PycharmProjects\EmailSend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlos.pepato\PycharmProjects\EmailSend\planilha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8845FE-3231-43C1-BCF8-5A81A83C577C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D037DF-BADF-468F-AF5D-04237497628A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{460DE964-D2E6-472C-B596-BE86DD347281}"/>
   </bookViews>
@@ -164,10 +164,10 @@
     <t>carlos.pepato@hi-mix.com.br; kadubelber1@gmail.com</t>
   </si>
   <si>
-    <t>kadubelber1@gmail.com</t>
-  </si>
-  <si>
     <t>carlos.pepato@hi-mix.com.br</t>
+  </si>
+  <si>
+    <t>matheus.felipe@hi-mix.com.br</t>
   </si>
 </sst>
 </file>
@@ -298,9 +298,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -338,7 +338,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -444,7 +444,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -586,7 +586,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -594,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BC2E975-7B4A-4775-B529-EDEF8E1CDC8C}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A2:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,44 +610,24 @@
     <col min="6" max="6" width="54" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="5">
-        <v>-8040.04</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -655,13 +635,13 @@
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="5">
-        <v>-57240</v>
+        <v>-8040.04</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>9</v>
@@ -675,13 +655,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="5">
-        <v>-103.5</v>
+        <v>-57240</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>9</v>
@@ -695,13 +675,13 @@
         <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="5">
-        <v>-295.2</v>
+        <v>-103.5</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>9</v>
@@ -715,13 +695,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="5">
-        <v>-58.2</v>
+        <v>-295.2</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>9</v>
@@ -735,13 +715,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="5">
-        <v>-29.4</v>
+        <v>-58.2</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>9</v>
@@ -755,13 +735,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="5">
-        <v>-371.52</v>
+        <v>-29.4</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>9</v>
@@ -775,13 +755,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="5">
-        <v>-220.5</v>
+        <v>-371.52</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>9</v>
@@ -795,13 +775,13 @@
         <v>6</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="5">
-        <v>-1502.28</v>
+        <v>-220.5</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>9</v>
@@ -815,13 +795,13 @@
         <v>6</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="5">
-        <v>-541.79999999999995</v>
+        <v>-1502.28</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>9</v>
@@ -835,13 +815,13 @@
         <v>6</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="5">
-        <v>-681</v>
+        <v>-541.79999999999995</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>9</v>
@@ -855,13 +835,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D13" s="5">
-        <v>-96162.31</v>
+        <v>-681</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>9</v>
@@ -872,22 +852,22 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="5">
-        <v>-2184</v>
+        <v>-96162.31</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -895,19 +875,19 @@
         <v>21</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="5">
-        <v>-612</v>
+        <v>-2184</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -915,19 +895,19 @@
         <v>21</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="5">
-        <v>-392</v>
+        <v>-612</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -935,33 +915,33 @@
         <v>21</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D17" s="5">
-        <v>-53480.08</v>
+        <v>-392</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D18" s="5">
-        <v>-234.96</v>
+        <v>-53480.08</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>9</v>
@@ -975,19 +955,19 @@
         <v>26</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D19" s="5">
-        <v>-26.99</v>
+        <v>-234.96</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -995,19 +975,19 @@
         <v>26</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D20" s="5">
-        <v>-242.8</v>
+        <v>-26.99</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1015,19 +995,19 @@
         <v>26</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="5">
-        <v>-6.99</v>
+        <v>-242.8</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1035,19 +1015,19 @@
         <v>26</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D22" s="5">
-        <v>-104.04</v>
+        <v>-6.99</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1055,19 +1035,19 @@
         <v>26</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D23" s="5">
-        <v>-244.46</v>
+        <v>-104.04</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1075,19 +1055,19 @@
         <v>26</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D24" s="5">
-        <v>-1385</v>
+        <v>-244.46</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1095,19 +1075,19 @@
         <v>26</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D25" s="5">
-        <v>-6.99</v>
+        <v>-1385</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1115,19 +1095,19 @@
         <v>26</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D26" s="5">
-        <v>-3984.32</v>
+        <v>-6.99</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1135,19 +1115,19 @@
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D27" s="5">
-        <v>-6.99</v>
+        <v>-3984.32</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1155,33 +1135,33 @@
         <v>26</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D28" s="5">
-        <v>-7.95</v>
+        <v>-6.99</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D29" s="5">
-        <v>-40328.230000000003</v>
+        <v>-7.95</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>9</v>
@@ -1195,19 +1175,39 @@
         <v>38</v>
       </c>
       <c r="B30" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="5">
+        <v>-40328.230000000003</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="5">
+      <c r="C31" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="5">
         <v>-34511.96</v>
       </c>
-      <c r="E30" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>42</v>
+      <c r="E31" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>